<commit_message>
refact:chartable  cost 컬럼 추가
</commit_message>
<xml_diff>
--- a/Document/GameTable/Character/SoldierCharTable.xlsx
+++ b/Document/GameTable/Character/SoldierCharTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ\Documents\Unreal Projects\ProjectBS\Document\GameTable\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15322D36-0333-484D-9558-CD8F83ADEADF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F800EF0D-8463-4BA6-AD93-8F3290DE8981}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{86F341D8-68CA-4ACF-86A3-A401C6774650}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,6 +80,10 @@
   </si>
   <si>
     <t>Id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cost</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1038,16 +1042,16 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" customWidth="1"/>
     <col min="4" max="4" width="15.25" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="19.75" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.875" customWidth="1"/>
     <col min="7" max="7" width="11.875" customWidth="1"/>
   </cols>
@@ -1068,6 +1072,9 @@
       <c r="E1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1086,6 +1093,9 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1103,7 +1113,9 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>300</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1121,7 +1133,9 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>500</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>

</xml_diff>